<commit_message>
Adjust test on _make_route
</commit_message>
<xml_diff>
--- a/tests/test_data/fwt_case5.xlsx
+++ b/tests/test_data/fwt_case5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{F390F16B-2CCF-41A4-B1CF-58362352A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6769AE1B-6249-4CCF-8D57-A789EA7EED24}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{F390F16B-2CCF-41A4-B1CF-58362352A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E11458C-D361-43C7-BD1D-906420B5DFCE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2FBD1F4-2459-45CD-802C-891B8518D02E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2FBD1F4-2459-45CD-802C-891B8518D02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,15 +529,16 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -587,7 +588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44950</v>
       </c>
@@ -634,9 +635,9 @@
         <v>769.12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44950</v>
+        <v>44951</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -681,7 +682,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44950</v>
       </c>
@@ -728,7 +729,7 @@
         <v>769.12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44950</v>
       </c>

</xml_diff>